<commit_message>
Retrained models, did RFE on the LR and RF
</commit_message>
<xml_diff>
--- a/Metrics/LoadedTestingMetrics.xlsx
+++ b/Metrics/LoadedTestingMetrics.xlsx
@@ -497,22 +497,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.266</v>
+        <v>0.318</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.059</v>
+        <v>0.016</v>
       </c>
       <c r="D3" t="n">
-        <v>0.465</v>
+        <v>0.433</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6820000000000001</v>
+        <v>0.658</v>
       </c>
       <c r="F3" t="n">
-        <v>0.763</v>
+        <v>0.766</v>
       </c>
       <c r="G3" t="n">
-        <v>0.555</v>
+        <v>0.591</v>
       </c>
     </row>
     <row r="4">
@@ -522,22 +522,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.196</v>
+        <v>-0.04</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.16</v>
+        <v>-0.5</v>
       </c>
       <c r="D4" t="n">
-        <v>0.51</v>
+        <v>0.66</v>
       </c>
       <c r="E4" t="n">
-        <v>0.714</v>
+        <v>0.8120000000000001</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6929999999999999</v>
+        <v>0.848</v>
       </c>
       <c r="G4" t="n">
-        <v>0.45</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="5">
@@ -547,22 +547,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.23</v>
+        <v>-0.046</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.519</v>
+        <v>-0.292</v>
       </c>
       <c r="D5" t="n">
-        <v>0.702</v>
+        <v>0.597</v>
       </c>
       <c r="E5" t="n">
-        <v>0.838</v>
+        <v>0.773</v>
       </c>
       <c r="F5" t="n">
-        <v>0.788</v>
+        <v>0.753</v>
       </c>
       <c r="G5" t="n">
-        <v>0.285</v>
+        <v>0.372</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New models trained, updated server main
</commit_message>
<xml_diff>
--- a/Metrics/LoadedTestingMetrics.xlsx
+++ b/Metrics/LoadedTestingMetrics.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -497,22 +497,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.318</v>
+        <v>0.261</v>
       </c>
       <c r="C3" t="n">
-        <v>0.016</v>
+        <v>-0.066</v>
       </c>
       <c r="D3" t="n">
-        <v>0.433</v>
+        <v>0.469</v>
       </c>
       <c r="E3" t="n">
-        <v>0.658</v>
+        <v>0.6850000000000001</v>
       </c>
       <c r="F3" t="n">
-        <v>0.766</v>
+        <v>0.769</v>
       </c>
       <c r="G3" t="n">
-        <v>0.591</v>
+        <v>0.5570000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -522,22 +522,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.04</v>
+        <v>0.193</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.5</v>
+        <v>-0.164</v>
       </c>
       <c r="D4" t="n">
-        <v>0.66</v>
+        <v>0.512</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8120000000000001</v>
+        <v>0.716</v>
       </c>
       <c r="F4" t="n">
-        <v>0.848</v>
+        <v>0.741</v>
       </c>
       <c r="G4" t="n">
-        <v>0.455</v>
+        <v>0.501</v>
       </c>
     </row>
     <row r="5">
@@ -547,22 +547,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.046</v>
+        <v>0.157</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.292</v>
+        <v>-0.041</v>
       </c>
       <c r="D5" t="n">
-        <v>0.597</v>
+        <v>0.481</v>
       </c>
       <c r="E5" t="n">
-        <v>0.773</v>
+        <v>0.694</v>
       </c>
       <c r="F5" t="n">
-        <v>0.753</v>
+        <v>0.6870000000000001</v>
       </c>
       <c r="G5" t="n">
-        <v>0.372</v>
+        <v>0.555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed residual plotting, added package used to requirements
</commit_message>
<xml_diff>
--- a/Metrics/LoadedTestingMetrics.xlsx
+++ b/Metrics/LoadedTestingMetrics.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Added ensemble model to main metric dictionary
</commit_message>
<xml_diff>
--- a/Metrics/LoadedTestingMetrics.xlsx
+++ b/Metrics/LoadedTestingMetrics.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -565,6 +565,31 @@
         <v>0.512</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Ensemble</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.444</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.666</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.672</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.553</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>